<commit_message>
More fixes and updated template
</commit_message>
<xml_diff>
--- a/public/templates/test-template-all-metrics-multiple-sheets.xlsx
+++ b/public/templates/test-template-all-metrics-multiple-sheets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinoliya.grace\Desktop\EmpAPPv1\employee-app-report-master\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinoliya.grace\Desktop\EmpAPPv1\prod_emp_app_report\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBFFF3A-6BE8-4C5A-BAD7-C512869CDF67}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78DFA79-81D0-42C2-80F2-46FC858C2473}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="834" firstSheet="19" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="834" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="App Installs - 7 Days" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="241">
   <si>
     <t>iOS</t>
   </si>
@@ -725,15 +725,6 @@
     <t>${table:saves6.total}</t>
   </si>
   <si>
-    <t>${table:sessionsavg7.total}</t>
-  </si>
-  <si>
-    <t>${table:sessionsavg30.total}</t>
-  </si>
-  <si>
-    <t>${table:sessionsavg6.total}</t>
-  </si>
-  <si>
     <t>${table:sessionsavg7.totalAvg}</t>
   </si>
   <si>
@@ -746,73 +737,37 @@
     <t>${table:docsreadavg7.totalAvg}</t>
   </si>
   <si>
-    <t>${table:docsreadavg7.total}</t>
-  </si>
-  <si>
     <t>${table:docsreadavg30.totalAvg}</t>
   </si>
   <si>
-    <t>${table:docsreadavg30.total}</t>
-  </si>
-  <si>
     <t>${table:articlesreadavg6.totalAvg}</t>
   </si>
   <si>
-    <t>${table:articlesreadavg6.total}</t>
-  </si>
-  <si>
     <t>${table:sharesavg7.totalAvg}</t>
   </si>
   <si>
-    <t>${table:sharesavg7.total}</t>
-  </si>
-  <si>
     <t>${table:sharesavg30.totalAvg}</t>
   </si>
   <si>
-    <t>${table:sharesavg30.total}</t>
-  </si>
-  <si>
     <t>${table:sharesavg6.totalAvg}</t>
   </si>
   <si>
-    <t>${table:sharesavg6.total}</t>
-  </si>
-  <si>
     <t>${table:commentsavg7.totalAvg}</t>
   </si>
   <si>
-    <t>${table:commentsavg7.total}</t>
-  </si>
-  <si>
     <t>${table:commentsavg30.totalAvg}</t>
   </si>
   <si>
-    <t>${table:commentsavg30.total}</t>
-  </si>
-  <si>
     <t>${table:commentsavg6.totalAvg}</t>
   </si>
   <si>
-    <t>${table:commentsavg6.total}</t>
-  </si>
-  <si>
     <t>${table:savesavg7.totalAvg}</t>
   </si>
   <si>
-    <t>${table:savesavg7.total}</t>
-  </si>
-  <si>
     <t>${table:savesavg30.totalAvg}</t>
   </si>
   <si>
-    <t>${table:savesavg30.total}</t>
-  </si>
-  <si>
     <t>${table:savesavg6.totalAvg}</t>
-  </si>
-  <si>
-    <t>${table:savesavg6.total}</t>
   </si>
   <si>
     <t>${table:topdocs30Date.daterange}</t>
@@ -828,9 +783,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-C09]d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-C09]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -1072,12 +1028,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1619,7 +1575,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1666,7 +1622,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1717,7 +1673,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2009,7 +1965,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2056,7 +2012,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2107,7 +2063,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2425,7 +2381,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2472,7 +2428,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2523,7 +2479,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2849,7 +2805,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2896,7 +2852,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2947,7 +2903,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3257,7 +3213,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3304,7 +3260,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3355,7 +3311,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3853,7 +3809,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3900,7 +3856,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3951,7 +3907,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4249,7 +4205,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4296,7 +4252,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4347,7 +4303,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4645,7 +4601,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4692,7 +4648,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4743,7 +4699,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5043,7 +4999,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5090,7 +5046,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5141,7 +5097,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5449,7 +5405,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5496,7 +5452,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5547,7 +5503,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6049,7 +6005,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6096,7 +6052,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6147,7 +6103,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6465,7 +6421,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6512,7 +6468,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6563,7 +6519,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6873,7 +6829,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6920,7 +6876,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6971,7 +6927,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7281,7 +7237,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -7328,7 +7284,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -7379,7 +7335,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8277,7 +8233,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -8324,7 +8280,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00">
+                <c:pt idx="0" formatCode="0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -8375,7 +8331,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -10496,13 +10452,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
+      <xdr:colOff>6351</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -11013,14 +10969,14 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="5" width="21.25" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="16.75" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.25" customWidth="1"/>
     <col min="13" max="13" width="17.375" customWidth="1"/>
     <col min="14" max="14" width="15.125" customWidth="1"/>
   </cols>
@@ -11032,7 +10988,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -11057,11 +11013,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>41</v>
       </c>
@@ -11077,17 +11030,14 @@
       <c r="H22" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>230</v>
+      <c r="K22" s="21" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -11104,7 +11054,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11113,7 +11063,7 @@
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="1.75" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.625" customWidth="1"/>
     <col min="13" max="13" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11124,7 +11074,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -11149,11 +11099,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>44</v>
       </c>
@@ -11169,17 +11116,14 @@
       <c r="H22" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>232</v>
+      <c r="K22" s="21" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -11196,7 +11140,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11205,7 +11149,7 @@
     <col min="6" max="6" width="8.625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="16.25" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.25" customWidth="1"/>
     <col min="13" max="13" width="17.25" customWidth="1"/>
     <col min="14" max="14" width="16.125" customWidth="1"/>
   </cols>
@@ -11217,7 +11161,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -11242,11 +11186,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>38</v>
       </c>
@@ -11262,17 +11203,14 @@
       <c r="H22" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>234</v>
+      <c r="K22" s="21" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -11289,7 +11227,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11299,7 +11237,7 @@
     <col min="7" max="7" width="7.625" customWidth="1"/>
     <col min="8" max="10" width="21.25" customWidth="1"/>
     <col min="11" max="11" width="21.375" customWidth="1"/>
-    <col min="12" max="12" width="17.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
     <col min="13" max="13" width="16.625" customWidth="1"/>
     <col min="14" max="14" width="15.5" customWidth="1"/>
   </cols>
@@ -11311,7 +11249,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -11336,11 +11274,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>47</v>
       </c>
@@ -11356,17 +11291,14 @@
       <c r="H22" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>236</v>
+      <c r="K22" s="21" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -11384,7 +11316,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11394,7 +11326,7 @@
     <col min="8" max="8" width="21.25" customWidth="1"/>
     <col min="9" max="9" width="21.25" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="16.75" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.875" customWidth="1"/>
     <col min="13" max="13" width="14.875" customWidth="1"/>
     <col min="14" max="14" width="15.75" customWidth="1"/>
   </cols>
@@ -11406,7 +11338,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -11431,11 +11363,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>50</v>
       </c>
@@ -11451,17 +11380,14 @@
       <c r="H22" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>238</v>
+      <c r="K22" s="21" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -11478,7 +11404,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11486,7 +11412,7 @@
     <col min="2" max="5" width="21.25" customWidth="1"/>
     <col min="6" max="6" width="9.25" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="15.125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
     <col min="13" max="13" width="16.125" customWidth="1"/>
     <col min="14" max="14" width="15.125" customWidth="1"/>
   </cols>
@@ -11498,7 +11424,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -11523,11 +11449,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>53</v>
       </c>
@@ -11543,17 +11466,14 @@
       <c r="H22" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>239</v>
-      </c>
-      <c r="L22" s="18" t="s">
-        <v>240</v>
+      <c r="K22" s="21" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -11570,7 +11490,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11579,7 +11499,7 @@
     <col min="6" max="6" width="8.75" customWidth="1"/>
     <col min="7" max="7" width="8.625" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="17.875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.875" customWidth="1"/>
     <col min="13" max="13" width="17.5" customWidth="1"/>
     <col min="14" max="14" width="14.125" customWidth="1"/>
   </cols>
@@ -11591,7 +11511,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -11616,11 +11536,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>56</v>
       </c>
@@ -11636,17 +11553,14 @@
       <c r="H22" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="K22" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>242</v>
+      <c r="K22" s="22" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -11663,7 +11577,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11674,7 +11588,7 @@
     <col min="6" max="6" width="9.25" customWidth="1"/>
     <col min="7" max="7" width="8.875" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="16" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="17.125" customWidth="1"/>
     <col min="14" max="14" width="16.75" customWidth="1"/>
   </cols>
@@ -11686,7 +11600,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -11711,11 +11625,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>59</v>
       </c>
@@ -11731,17 +11642,14 @@
       <c r="H22" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>243</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>244</v>
+      <c r="K22" s="21" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -11759,7 +11667,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11770,7 +11678,7 @@
     <col min="8" max="9" width="21.25" customWidth="1"/>
     <col min="10" max="10" width="21.125" customWidth="1"/>
     <col min="11" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="17.125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.625" customWidth="1"/>
     <col min="13" max="13" width="17.25" customWidth="1"/>
     <col min="14" max="14" width="18.375" customWidth="1"/>
   </cols>
@@ -11782,7 +11690,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -11807,11 +11715,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>62</v>
       </c>
@@ -11827,17 +11732,14 @@
       <c r="H22" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>246</v>
+      <c r="K22" s="21" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -11854,7 +11756,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11863,7 +11765,7 @@
     <col min="6" max="6" width="8.125" customWidth="1"/>
     <col min="7" max="7" width="7.25" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="16.875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.875" customWidth="1"/>
     <col min="13" max="13" width="17.125" customWidth="1"/>
     <col min="14" max="14" width="15.25" customWidth="1"/>
   </cols>
@@ -11875,7 +11777,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -11900,11 +11802,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>65</v>
       </c>
@@ -11920,17 +11819,14 @@
       <c r="H22" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>248</v>
+      <c r="K22" s="21" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -12009,8 +11905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019AF990-9EF1-4B5A-A561-52A55C330FE5}">
   <dimension ref="B2:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -12019,7 +11915,7 @@
     <col min="6" max="6" width="8.875" customWidth="1"/>
     <col min="7" max="7" width="7.625" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="16.625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" customWidth="1"/>
     <col min="13" max="13" width="16.625" customWidth="1"/>
     <col min="14" max="14" width="14.625" customWidth="1"/>
   </cols>
@@ -12031,7 +11927,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -12056,11 +11952,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>68</v>
       </c>
@@ -12076,17 +11969,14 @@
       <c r="H22" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>249</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>250</v>
+      <c r="K22" s="21" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -12103,7 +11993,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -12112,7 +12002,7 @@
     <col min="6" max="6" width="8.75" customWidth="1"/>
     <col min="7" max="7" width="8.625" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="17.625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.25" customWidth="1"/>
     <col min="13" max="13" width="18.25" customWidth="1"/>
     <col min="14" max="14" width="12.625" customWidth="1"/>
   </cols>
@@ -12124,7 +12014,7 @@
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -12149,11 +12039,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>71</v>
       </c>
@@ -12169,17 +12056,14 @@
       <c r="H22" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>251</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>252</v>
+      <c r="K22" s="21" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -12300,7 +12184,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="C1" s="26" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="D1" s="23"/>
     </row>
@@ -12389,7 +12273,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="26" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C1" s="23"/>
     </row>
@@ -12551,7 +12435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E264C6-F834-4EFB-AAE0-C549A2ACBA95}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -12565,7 +12449,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="26" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C1" s="23"/>
     </row>
@@ -12727,7 +12611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -12852,7 +12736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -12980,10 +12864,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B2:L22"/>
+  <dimension ref="B2:K22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -12992,7 +12876,7 @@
     <col min="6" max="6" width="9.75" customWidth="1"/>
     <col min="7" max="7" width="9.125" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -13008,7 +12892,7 @@
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -13033,11 +12917,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
@@ -13053,16 +12934,13 @@
       <c r="H22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="L22" s="1" t="s">
+      <c r="K22" s="21" t="s">
         <v>223</v>
       </c>
     </row>
@@ -13095,7 +12973,7 @@
     <col min="6" max="6" width="10.375" customWidth="1"/>
     <col min="7" max="7" width="9.125" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -13107,9 +12985,9 @@
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
     </row>
     <row r="21" spans="2:12">
       <c r="B21" s="2" t="s">
@@ -13136,9 +13014,6 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
     </row>
     <row r="22" spans="2:12">
       <c r="B22" s="7" t="s">
@@ -13156,192 +13031,189 @@
       <c r="H22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="L22" s="19" t="s">
+      <c r="K22" s="21" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="23" spans="2:12">
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
     </row>
     <row r="25" spans="2:12">
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
     </row>
     <row r="26" spans="2:12">
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
     </row>
     <row r="27" spans="2:12">
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
     </row>
     <row r="28" spans="2:12">
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
     </row>
     <row r="29" spans="2:12">
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
     </row>
     <row r="30" spans="2:12">
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
     </row>
     <row r="31" spans="2:12">
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
     </row>
     <row r="32" spans="2:12">
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
     </row>
     <row r="33" spans="9:12">
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
     </row>
     <row r="34" spans="9:12">
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
     </row>
     <row r="35" spans="9:12">
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
     </row>
     <row r="36" spans="9:12">
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
     </row>
     <row r="37" spans="9:12">
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
     </row>
     <row r="38" spans="9:12">
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
     </row>
     <row r="39" spans="9:12">
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
     </row>
     <row r="40" spans="9:12">
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
     </row>
     <row r="41" spans="9:12">
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
     </row>
     <row r="42" spans="9:12">
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
     </row>
     <row r="43" spans="9:12">
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
     </row>
     <row r="44" spans="9:12">
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
     </row>
     <row r="45" spans="9:12">
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
     </row>
     <row r="46" spans="9:12">
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="20"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
     </row>
     <row r="47" spans="9:12">
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
     </row>
     <row r="48" spans="9:12">
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="20"/>
-      <c r="L48" s="20"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
     </row>
     <row r="49" spans="9:12">
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-      <c r="K49" s="20"/>
-      <c r="L49" s="20"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19"/>
     </row>
     <row r="50" spans="9:12">
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
     </row>
     <row r="51" spans="9:12">
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13363,7 +13235,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -13372,7 +13244,7 @@
     <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="10.375" customWidth="1"/>
     <col min="8" max="11" width="21.25" customWidth="1"/>
-    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -13388,7 +13260,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" s="2" t="s">
         <v>195</v>
       </c>
@@ -13413,11 +13285,8 @@
       <c r="K21" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
         <v>32</v>
       </c>
@@ -13433,16 +13302,13 @@
       <c r="H22" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="K22" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="L22" s="1" t="s">
+      <c r="K22" s="21" t="s">
         <v>225</v>
       </c>
     </row>

</xml_diff>